<commit_message>
Merge my work into ADAPT_Blueprint.xlsx
</commit_message>
<xml_diff>
--- a/Lab_5/ADAPT_Blueprint.xlsx
+++ b/Lab_5/ADAPT_Blueprint.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nap/Documents/Junior2/Software Engineering/Lab5SoftEngineer/Lab_5/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanchanokkinra/Documents/SoftEngineer/Lab5SoftEngineer/Lab_5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB5129A2-8B4C-0D4F-BF51-84BC73FAD5DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B3C5FC-8B5E-7E47-BC10-EAF4F4A33D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C5F2AE7F-2A01-4E3D-A1FD-0F4756AFC920}"/>
+    <workbookView xWindow="0" yWindow="620" windowWidth="28800" windowHeight="16160" xr2:uid="{C5F2AE7F-2A01-4E3D-A1FD-0F4756AFC920}"/>
   </bookViews>
   <sheets>
     <sheet name="A-DAPT Blueprint" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="77">
   <si>
     <t>A-DAPT Blueprint</t>
   </si>
@@ -268,6 +268,60 @@
   </si>
   <si>
     <t>ไม่ (Login)</t>
+  </si>
+  <si>
+    <t>ตาราง Filter</t>
+  </si>
+  <si>
+    <t>Subject_Code</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>section</t>
+  </si>
+  <si>
+    <t>Enum</t>
+  </si>
+  <si>
+    <t>VarChar</t>
+  </si>
+  <si>
+    <t>Char</t>
+  </si>
+  <si>
+    <t>ตาราง Exam</t>
+  </si>
+  <si>
+    <t>field</t>
+  </si>
+  <si>
+    <t>academic_year</t>
+  </si>
+  <si>
+    <t>semster</t>
+  </si>
+  <si>
+    <t>Room</t>
+  </si>
+  <si>
+    <t>Start_time</t>
+  </si>
+  <si>
+    <t>End_time</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>varchar</t>
+  </si>
+  <si>
+    <t>time</t>
   </si>
 </sst>
 </file>
@@ -278,7 +332,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -286,7 +340,7 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -294,14 +348,14 @@
       <b/>
       <sz val="28"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -341,7 +395,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -349,12 +403,12 @@
       <b/>
       <sz val="18"/>
       <color theme="1" tint="0.499984740745262"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -379,6 +433,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -550,7 +610,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -640,6 +700,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -688,27 +766,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -783,14 +846,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>669924</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>14288</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1419754</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>4763</xdr:rowOff>
     </xdr:to>
@@ -807,8 +870,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="657225" y="1590675"/>
-          <a:ext cx="6481763" cy="4763"/>
+          <a:off x="669924" y="7755467"/>
+          <a:ext cx="14228763" cy="4763"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -840,15 +903,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>77258</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>372533</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>14288</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>4763</xdr:rowOff>
+      <xdr:colOff>82021</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>377296</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -863,8 +926,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="657225" y="4424363"/>
-          <a:ext cx="11149013" cy="4763"/>
+          <a:off x="754591" y="10464800"/>
+          <a:ext cx="14228763" cy="4763"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -976,7 +1039,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ธีม Office 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -1277,16 +1340,16 @@
   </sheetPr>
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="39" zoomScaleNormal="108" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="75" zoomScaleNormal="108" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
     <col min="2" max="11" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="37">
+    <row r="1" spans="1:11" ht="35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1426,67 +1489,67 @@
       <c r="B10" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="H10" s="55" t="e" vm="1">
+      <c r="H10" s="40" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="I10" s="55"/>
-      <c r="J10" s="55" t="e" vm="2">
+      <c r="I10" s="40"/>
+      <c r="J10" s="40" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
-      <c r="K10" s="59"/>
+      <c r="K10" s="43"/>
     </row>
     <row r="11" spans="1:11" ht="30" customHeight="1">
       <c r="A11" s="33"/>
-      <c r="B11" s="56" t="e" vm="3">
+      <c r="B11" s="39" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
-      <c r="C11" s="55"/>
-      <c r="D11" s="55" t="e" vm="4">
+      <c r="C11" s="40"/>
+      <c r="D11" s="40" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
-      <c r="E11" s="55"/>
-      <c r="H11" s="55"/>
-      <c r="I11" s="55"/>
-      <c r="J11" s="55"/>
-      <c r="K11" s="59"/>
+      <c r="E11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="40"/>
+      <c r="K11" s="43"/>
     </row>
     <row r="12" spans="1:11" ht="30" customHeight="1">
       <c r="A12" s="33"/>
-      <c r="B12" s="56"/>
-      <c r="C12" s="55"/>
-      <c r="D12" s="55"/>
-      <c r="E12" s="55"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
       <c r="G12" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="H12" s="55"/>
-      <c r="I12" s="55"/>
-      <c r="J12" s="55"/>
-      <c r="K12" s="59"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="40"/>
+      <c r="K12" s="43"/>
     </row>
     <row r="13" spans="1:11" ht="30" customHeight="1">
       <c r="A13" s="33"/>
-      <c r="B13" s="56"/>
-      <c r="C13" s="55"/>
-      <c r="D13" s="55"/>
-      <c r="E13" s="55"/>
-      <c r="H13" s="55"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="55"/>
-      <c r="K13" s="59"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="43"/>
     </row>
     <row r="14" spans="1:11" ht="30" customHeight="1">
       <c r="A14" s="34"/>
-      <c r="B14" s="57"/>
-      <c r="C14" s="58"/>
-      <c r="D14" s="58"/>
-      <c r="E14" s="58"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
-      <c r="H14" s="58"/>
-      <c r="I14" s="58"/>
-      <c r="J14" s="58"/>
-      <c r="K14" s="60"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="42"/>
+      <c r="K14" s="44"/>
     </row>
     <row r="15" spans="1:11" ht="30" customHeight="1">
       <c r="A15" s="35" t="s">
@@ -1526,37 +1589,97 @@
       <c r="B20" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="K20" s="4"/>
+      <c r="G20" s="61" t="s">
+        <v>59</v>
+      </c>
+      <c r="H20" s="61"/>
+      <c r="I20" s="62"/>
+      <c r="J20" s="61" t="s">
+        <v>66</v>
+      </c>
+      <c r="K20" s="63"/>
     </row>
     <row r="21" spans="1:11" ht="30" customHeight="1">
       <c r="A21" s="35"/>
-      <c r="K21" s="4"/>
+      <c r="G21" s="61" t="s">
+        <v>60</v>
+      </c>
+      <c r="H21" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="I21" s="62"/>
+      <c r="J21" s="61" t="s">
+        <v>67</v>
+      </c>
+      <c r="K21" s="63" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="22" spans="1:11" ht="30" customHeight="1">
       <c r="A22" s="35"/>
-      <c r="K22" s="4"/>
+      <c r="G22" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="H22" s="61" t="s">
+        <v>64</v>
+      </c>
+      <c r="I22" s="62"/>
+      <c r="J22" s="61" t="s">
+        <v>68</v>
+      </c>
+      <c r="K22" s="63" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="23" spans="1:11" ht="30" customHeight="1">
       <c r="A23" s="35"/>
-      <c r="K23" s="4"/>
+      <c r="G23" s="61" t="s">
+        <v>62</v>
+      </c>
+      <c r="H23" s="61" t="s">
+        <v>63</v>
+      </c>
+      <c r="I23" s="62"/>
+      <c r="J23" s="61" t="s">
+        <v>69</v>
+      </c>
+      <c r="K23" s="63" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="24" spans="1:11" ht="30" customHeight="1">
       <c r="A24" s="35"/>
-      <c r="K24" s="4"/>
+      <c r="J24" s="61" t="s">
+        <v>70</v>
+      </c>
+      <c r="K24" s="63" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="25" spans="1:11" ht="30" customHeight="1">
       <c r="A25" s="36"/>
-      <c r="B25" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="K25" s="4"/>
+      <c r="B25" s="12"/>
+      <c r="J25" s="61" t="s">
+        <v>71</v>
+      </c>
+      <c r="K25" s="63" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="26" spans="1:11" ht="30" customHeight="1">
       <c r="A26" s="35"/>
-      <c r="K26" s="4"/>
+      <c r="J26" s="61" t="s">
+        <v>72</v>
+      </c>
+      <c r="K26" s="63" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="27" spans="1:11" ht="30" customHeight="1">
       <c r="A27" s="35"/>
+      <c r="B27" s="11" t="s">
+        <v>7</v>
+      </c>
       <c r="K27" s="4"/>
     </row>
     <row r="28" spans="1:11" ht="30" customHeight="1">
@@ -1600,7 +1723,7 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="16.6640625" customWidth="1"/>
     <col min="2" max="2" width="21.83203125" customWidth="1"/>
@@ -1610,17 +1733,17 @@
     <col min="6" max="6" width="51.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="27">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:6" ht="23">
+      <c r="A1" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-    </row>
-    <row r="2" spans="1:6" ht="27">
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+    </row>
+    <row r="2" spans="1:6" ht="23">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -1628,53 +1751,53 @@
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
     </row>
-    <row r="3" spans="1:6" ht="27">
+    <row r="3" spans="1:6" ht="23">
       <c r="A3" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="48"/>
+      <c r="B3" s="53"/>
+      <c r="C3" s="54"/>
       <c r="D3" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="49"/>
-      <c r="F3" s="45"/>
-    </row>
-    <row r="4" spans="1:6" ht="27">
+      <c r="E3" s="55"/>
+      <c r="F3" s="51"/>
+    </row>
+    <row r="4" spans="1:6" ht="23">
       <c r="A4" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="43"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="49"/>
       <c r="D4" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="44"/>
-      <c r="F4" s="45"/>
-    </row>
-    <row r="5" spans="1:6" ht="27">
+      <c r="E4" s="50"/>
+      <c r="F4" s="51"/>
+    </row>
+    <row r="5" spans="1:6" ht="23">
       <c r="A5" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="49"/>
-      <c r="C5" s="44"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="50"/>
       <c r="D5" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="50"/>
-      <c r="F5" s="51"/>
-    </row>
-    <row r="6" spans="1:6" ht="27">
-      <c r="A6" s="52" t="s">
+      <c r="E5" s="56"/>
+      <c r="F5" s="57"/>
+    </row>
+    <row r="6" spans="1:6" ht="23">
+      <c r="A6" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="52"/>
-      <c r="C6" s="49"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="45"/>
-    </row>
-    <row r="7" spans="1:6" ht="27">
+      <c r="B6" s="58"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="51"/>
+    </row>
+    <row r="7" spans="1:6" ht="23">
       <c r="A7" s="13"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -1702,32 +1825,32 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="27">
-      <c r="A9" s="39"/>
+    <row r="9" spans="1:6" ht="23">
+      <c r="A9" s="45"/>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
     </row>
-    <row r="10" spans="1:6" ht="27">
-      <c r="A10" s="40"/>
+    <row r="10" spans="1:6" ht="23">
+      <c r="A10" s="46"/>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
     </row>
-    <row r="11" spans="1:6" ht="27">
-      <c r="A11" s="40"/>
+    <row r="11" spans="1:6" ht="23">
+      <c r="A11" s="46"/>
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
     </row>
-    <row r="12" spans="1:6" ht="27">
-      <c r="A12" s="41"/>
+    <row r="12" spans="1:6" ht="23">
+      <c r="A12" s="47"/>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
@@ -1819,10 +1942,10 @@
       <c r="C9" s="19"/>
     </row>
     <row r="10" spans="1:3" ht="30" customHeight="1">
-      <c r="A10" s="53" t="s">
+      <c r="A10" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="54"/>
+      <c r="B10" s="60"/>
       <c r="C10" s="20"/>
     </row>
   </sheetData>
@@ -1841,7 +1964,7 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="27"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="23"/>
   <cols>
     <col min="1" max="1" width="16.6640625" style="13" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" style="13" customWidth="1"/>

</xml_diff>

<commit_message>
Update ADAPT Blueprint (Data Base Login)
</commit_message>
<xml_diff>
--- a/Lab_5/ADAPT_Blueprint.xlsx
+++ b/Lab_5/ADAPT_Blueprint.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NBODT\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Lab5SoftEngineer\Lab_5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{847AAA3F-5D23-4544-BE03-AFE6DE69283D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A885290-A6F1-4C24-9108-659FEB28A510}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{C5F2AE7F-2A01-4E3D-A1FD-0F4756AFC920}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{C5F2AE7F-2A01-4E3D-A1FD-0F4756AFC920}"/>
   </bookViews>
   <sheets>
     <sheet name="A-DAPT Blueprint" sheetId="1" r:id="rId1"/>
@@ -26,12 +26,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +34,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
@@ -91,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="130">
   <si>
     <t>A-DAPT Blueprint</t>
   </si>
@@ -298,9 +293,6 @@
   </si>
   <si>
     <t>academic_year</t>
-  </si>
-  <si>
-    <t>semster</t>
   </si>
   <si>
     <t>Room</t>
@@ -451,16 +443,64 @@
 4.ชื่อวิชาควรกรอกให้ครบจะเป็นชื่อตัวพิมพ์ใหญ่หรือเล็กก็ได้
 5. Section เป็นตัวเลขอย่างเดียว</t>
   </si>
+  <si>
+    <t>ตาราง User</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>STd_Id</t>
+  </si>
+  <si>
+    <t>national_Id</t>
+  </si>
+  <si>
+    <t>VARCHAR</t>
+  </si>
+  <si>
+    <t>unique</t>
+  </si>
+  <si>
+    <t>char(68)</t>
+  </si>
+  <si>
+    <t>hash(sha256)</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>academicyear</t>
+  </si>
+  <si>
+    <t>semester</t>
+  </si>
+  <si>
+    <t>room</t>
+  </si>
+  <si>
+    <t>staAT_time</t>
+  </si>
+  <si>
+    <t>ตารางวิชาเรียน</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>char</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -468,7 +508,7 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -476,14 +516,14 @@
       <b/>
       <sz val="28"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -523,7 +563,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -531,7 +571,7 @@
       <b/>
       <sz val="18"/>
       <color theme="1" tint="0.499984740745262"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -568,7 +608,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -792,17 +832,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
@@ -834,19 +863,21 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -915,17 +946,12 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -933,123 +959,15 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1061,9 +979,135 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1252,7 +1296,7 @@
 </file>
 
 <file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
-<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
   <global>
     <keyFlags>
       <key name="_Self">
@@ -1331,9 +1375,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ธีม Office 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1371,7 +1415,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1477,7 +1521,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1619,7 +1663,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1632,24 +1676,24 @@
   </sheetPr>
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="96" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="11" width="18.6328125" customWidth="1"/>
-    <col min="12" max="12" width="17.6328125" customWidth="1"/>
-    <col min="13" max="13" width="17.54296875" customWidth="1"/>
-    <col min="14" max="14" width="17.6328125" customWidth="1"/>
+    <col min="2" max="11" width="18.625" customWidth="1"/>
+    <col min="12" max="12" width="17.625" customWidth="1"/>
+    <col min="13" max="13" width="17.5" customWidth="1"/>
+    <col min="14" max="14" width="17.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="36">
+    <row r="1" spans="1:14" ht="34.5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="50" customHeight="1">
+    <row r="2" spans="1:14" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -1670,7 +1714,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="50" customHeight="1">
+    <row r="3" spans="1:14" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
@@ -1684,13 +1728,13 @@
       <c r="I3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="54" t="s">
+      <c r="J3" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="55"/>
-    </row>
-    <row r="5" spans="1:14" ht="30" customHeight="1">
-      <c r="A5" s="49" t="s">
+      <c r="K3" s="57"/>
+    </row>
+    <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="51" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="10" t="s">
@@ -1712,8 +1756,8 @@
       <c r="J5" s="2"/>
       <c r="K5" s="3"/>
     </row>
-    <row r="6" spans="1:14" ht="30" customHeight="1">
-      <c r="A6" s="50"/>
+    <row r="6" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="52"/>
       <c r="B6" s="27" t="s">
         <v>39</v>
       </c>
@@ -1728,8 +1772,8 @@
       </c>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:14" ht="30" customHeight="1">
-      <c r="A7" s="50"/>
+    <row r="7" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="52"/>
       <c r="B7" s="25" t="s">
         <v>40</v>
       </c>
@@ -1747,8 +1791,8 @@
       </c>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="1:14" ht="30" customHeight="1">
-      <c r="A8" s="50"/>
+    <row r="8" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="52"/>
       <c r="B8" s="26" t="s">
         <v>41</v>
       </c>
@@ -1763,8 +1807,8 @@
       </c>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="1:14" ht="30" customHeight="1">
-      <c r="A9" s="50"/>
+    <row r="9" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="52"/>
       <c r="B9" s="26" t="s">
         <v>42</v>
       </c>
@@ -1779,337 +1823,442 @@
       </c>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="1:14" ht="30" customHeight="1">
-      <c r="A10" s="50"/>
+    <row r="10" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="52"/>
       <c r="B10" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="H10" s="57" t="e" vm="1">
+      <c r="H10" s="59" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="I10" s="57"/>
-      <c r="J10" s="57" t="e" vm="2">
+      <c r="I10" s="59"/>
+      <c r="J10" s="59" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
-      <c r="K10" s="60"/>
-    </row>
-    <row r="11" spans="1:14" ht="30" customHeight="1">
-      <c r="A11" s="50"/>
-      <c r="B11" s="56" t="e" vm="3">
+      <c r="K10" s="62"/>
+    </row>
+    <row r="11" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="52"/>
+      <c r="B11" s="58" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
-      <c r="C11" s="57"/>
-      <c r="D11" s="57" t="e" vm="4">
+      <c r="C11" s="59"/>
+      <c r="D11" s="59" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
-      <c r="E11" s="57"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="57"/>
-      <c r="J11" s="57"/>
-      <c r="K11" s="60"/>
-    </row>
-    <row r="12" spans="1:14" ht="30" customHeight="1">
-      <c r="A12" s="50"/>
-      <c r="B12" s="56"/>
-      <c r="C12" s="57"/>
-      <c r="D12" s="57"/>
-      <c r="E12" s="57"/>
+      <c r="E11" s="59"/>
+      <c r="H11" s="59"/>
+      <c r="I11" s="59"/>
+      <c r="J11" s="59"/>
+      <c r="K11" s="62"/>
+    </row>
+    <row r="12" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="52"/>
+      <c r="B12" s="58"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="59"/>
       <c r="G12" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="H12" s="57"/>
-      <c r="I12" s="57"/>
-      <c r="J12" s="57"/>
-      <c r="K12" s="60"/>
-    </row>
-    <row r="13" spans="1:14" ht="30" customHeight="1">
-      <c r="A13" s="50"/>
-      <c r="B13" s="56"/>
-      <c r="C13" s="57"/>
-      <c r="D13" s="57"/>
-      <c r="E13" s="57"/>
-      <c r="H13" s="57"/>
-      <c r="I13" s="57"/>
-      <c r="J13" s="57"/>
-      <c r="K13" s="60"/>
-    </row>
-    <row r="14" spans="1:14" ht="30" customHeight="1" thickBot="1">
-      <c r="A14" s="51"/>
-      <c r="B14" s="58"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="57"/>
-      <c r="H14" s="57"/>
-      <c r="I14" s="59"/>
-      <c r="J14" s="59"/>
-      <c r="K14" s="61"/>
-    </row>
-    <row r="15" spans="1:14" ht="30" customHeight="1" thickBot="1">
-      <c r="A15" s="52" t="s">
+      <c r="H12" s="59"/>
+      <c r="I12" s="59"/>
+      <c r="J12" s="59"/>
+      <c r="K12" s="62"/>
+    </row>
+    <row r="13" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="52"/>
+      <c r="B13" s="58"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="59"/>
+      <c r="H13" s="59"/>
+      <c r="I13" s="59"/>
+      <c r="J13" s="59"/>
+      <c r="K13" s="62"/>
+    </row>
+    <row r="14" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="53"/>
+      <c r="B14" s="60"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="59"/>
+      <c r="H14" s="59"/>
+      <c r="I14" s="61"/>
+      <c r="J14" s="61"/>
+      <c r="K14" s="63"/>
+    </row>
+    <row r="15" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="54" t="s">
         <v>4</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="46"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="35" t="s">
+      <c r="C15" s="42"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="F15" s="41"/>
+      <c r="G15" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="H15" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="I15" s="2"/>
+      <c r="J15" s="64" t="s">
+        <v>104</v>
+      </c>
+      <c r="K15" s="64" t="s">
+        <v>113</v>
+      </c>
+      <c r="L15" s="50" t="s">
+        <v>87</v>
+      </c>
+      <c r="M15" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="N15" s="46" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="55"/>
+      <c r="B16" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="E16" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="F15" s="45"/>
-      <c r="G15" s="39" t="s">
+      <c r="G16" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="H15" s="35" t="s">
+      <c r="H16" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="J16" s="65"/>
+      <c r="K16" s="66"/>
+      <c r="L16" s="47" t="s">
+        <v>105</v>
+      </c>
+      <c r="M16" s="47" t="s">
+        <v>107</v>
+      </c>
+      <c r="N16" s="47" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="55"/>
+      <c r="B17" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="E17" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="F17" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="G17" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="H17" s="34" t="s">
         <v>101</v>
-      </c>
-      <c r="I15" s="2"/>
-      <c r="J15" s="78" t="s">
-        <v>105</v>
-      </c>
-      <c r="K15" s="78" t="s">
-        <v>114</v>
-      </c>
-      <c r="L15" s="89" t="s">
-        <v>88</v>
-      </c>
-      <c r="M15" s="85" t="s">
-        <v>93</v>
-      </c>
-      <c r="N15" s="85" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="30" customHeight="1" thickBot="1">
-      <c r="A16" s="53"/>
-      <c r="B16" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="C16" s="35" t="s">
-        <v>80</v>
-      </c>
-      <c r="D16" s="39" t="s">
-        <v>82</v>
-      </c>
-      <c r="E16" s="37" t="s">
-        <v>89</v>
-      </c>
-      <c r="G16" s="41" t="s">
-        <v>97</v>
-      </c>
-      <c r="H16" s="36" t="s">
-        <v>89</v>
-      </c>
-      <c r="J16" s="83"/>
-      <c r="K16" s="79"/>
-      <c r="L16" s="86" t="s">
-        <v>106</v>
-      </c>
-      <c r="M16" s="86" t="s">
-        <v>108</v>
-      </c>
-      <c r="N16" s="86" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" ht="30" customHeight="1">
-      <c r="A17" s="53"/>
-      <c r="B17" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="C17" s="36" t="s">
-        <v>86</v>
-      </c>
-      <c r="D17" s="40" t="s">
-        <v>83</v>
-      </c>
-      <c r="E17" s="37" t="s">
-        <v>90</v>
-      </c>
-      <c r="F17" s="47" t="s">
-        <v>93</v>
-      </c>
-      <c r="G17" s="41" t="s">
-        <v>98</v>
-      </c>
-      <c r="H17" s="36" t="s">
-        <v>102</v>
       </c>
       <c r="I17" t="s">
         <v>58</v>
       </c>
-      <c r="J17" s="83"/>
-      <c r="K17" s="79"/>
-      <c r="L17" s="87" t="s">
-        <v>107</v>
-      </c>
-      <c r="M17" s="88" t="s">
-        <v>109</v>
-      </c>
-      <c r="N17" s="86" t="s">
+      <c r="J17" s="65"/>
+      <c r="K17" s="66"/>
+      <c r="L17" s="48" t="s">
+        <v>106</v>
+      </c>
+      <c r="M17" s="49" t="s">
+        <v>108</v>
+      </c>
+      <c r="N17" s="47" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="55"/>
+      <c r="B18" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="F18" s="40" t="s">
+        <v>93</v>
+      </c>
+      <c r="G18" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="H18" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="J18" s="65"/>
+      <c r="K18" s="67"/>
+      <c r="L18" s="44"/>
+      <c r="M18" s="45"/>
+      <c r="N18" s="47" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="30" customHeight="1" thickBot="1">
-      <c r="A18" s="53"/>
-      <c r="B18" s="43" t="s">
-        <v>79</v>
-      </c>
-      <c r="C18" s="37" t="s">
-        <v>87</v>
-      </c>
-      <c r="D18" s="41" t="s">
-        <v>85</v>
-      </c>
-      <c r="E18" s="36" t="s">
+    <row r="19" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="54"/>
+      <c r="C19" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="F18" s="44" t="s">
+      <c r="F19" s="96" t="s">
         <v>94</v>
       </c>
-      <c r="G18" s="41" t="s">
+      <c r="G19" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="H18" s="36" t="s">
+      <c r="H19" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="J18" s="83"/>
-      <c r="K18" s="80"/>
-      <c r="L18" s="81"/>
-      <c r="M18" s="82"/>
-      <c r="N18" s="86" t="s">
+      <c r="J19" s="65"/>
+      <c r="K19" s="67"/>
+      <c r="L19" s="44"/>
+      <c r="M19" s="45"/>
+      <c r="N19" s="47" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="30" customHeight="1" thickBot="1">
-      <c r="A19" s="52"/>
-      <c r="C19" s="38" t="s">
-        <v>81</v>
-      </c>
-      <c r="D19" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="E19" s="38" t="s">
-        <v>92</v>
-      </c>
-      <c r="F19" s="48" t="s">
-        <v>95</v>
-      </c>
-      <c r="G19" s="42" t="s">
-        <v>100</v>
-      </c>
-      <c r="H19" s="38" t="s">
-        <v>104</v>
-      </c>
-      <c r="J19" s="84"/>
-      <c r="K19" s="80"/>
-      <c r="L19" s="81"/>
-      <c r="M19" s="82"/>
-      <c r="N19" s="87" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" ht="30" customHeight="1">
-      <c r="A20" s="52"/>
+    <row r="20" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="54"/>
       <c r="B20" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G20" s="32" t="s">
+      <c r="C20" s="93" t="s">
+        <v>114</v>
+      </c>
+      <c r="D20" s="95"/>
+      <c r="E20" s="94"/>
+      <c r="F20" s="93" t="s">
+        <v>66</v>
+      </c>
+      <c r="G20" s="94"/>
+      <c r="H20" s="93" t="s">
+        <v>127</v>
+      </c>
+      <c r="I20" s="94"/>
+      <c r="J20" s="91"/>
+      <c r="K20" s="93" t="s">
         <v>59</v>
       </c>
-      <c r="H20" s="32"/>
-      <c r="J20" s="32" t="s">
+      <c r="L20" s="94"/>
+      <c r="M20" s="93" t="s">
         <v>66</v>
       </c>
-      <c r="K20" s="33"/>
-    </row>
-    <row r="21" spans="1:14" ht="30" customHeight="1">
-      <c r="A21" s="52"/>
-      <c r="G21" s="32" t="s">
+      <c r="N20" s="94"/>
+    </row>
+    <row r="21" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="54"/>
+      <c r="C21" s="86" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="89" t="s">
+        <v>122</v>
+      </c>
+      <c r="E21" s="89" t="s">
+        <v>115</v>
+      </c>
+      <c r="F21" s="84" t="s">
+        <v>67</v>
+      </c>
+      <c r="G21" s="97" t="s">
+        <v>122</v>
+      </c>
+      <c r="H21" s="84" t="s">
+        <v>128</v>
+      </c>
+      <c r="I21" s="85" t="s">
+        <v>72</v>
+      </c>
+      <c r="J21" s="92"/>
+      <c r="K21" s="86" t="s">
         <v>60</v>
       </c>
-      <c r="H21" s="32" t="s">
+      <c r="L21" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="J21" s="32" t="s">
+      <c r="M21" s="86" t="s">
         <v>67</v>
       </c>
-      <c r="K21" s="33" t="s">
+      <c r="N21" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="54"/>
+      <c r="C22" s="86" t="s">
+        <v>116</v>
+      </c>
+      <c r="D22" s="89" t="s">
+        <v>118</v>
+      </c>
+      <c r="E22" s="89" t="s">
+        <v>119</v>
+      </c>
+      <c r="F22" s="98" t="s">
+        <v>123</v>
+      </c>
+      <c r="G22" s="99" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" ht="30" customHeight="1">
-      <c r="A22" s="52"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="32" t="s">
+      <c r="H22" s="86" t="s">
+        <v>60</v>
+      </c>
+      <c r="I22" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="J22" s="92"/>
+      <c r="K22" s="86" t="s">
         <v>61</v>
       </c>
-      <c r="H22" s="32" t="s">
+      <c r="L22" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="J22" s="32" t="s">
+      <c r="M22" s="86" t="s">
         <v>68</v>
       </c>
-      <c r="K22" s="33" t="s">
+      <c r="N22" s="32" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="54"/>
+      <c r="C23" s="87" t="s">
+        <v>117</v>
+      </c>
+      <c r="D23" s="90" t="s">
+        <v>120</v>
+      </c>
+      <c r="E23" s="90" t="s">
+        <v>121</v>
+      </c>
+      <c r="F23" s="86" t="s">
+        <v>124</v>
+      </c>
+      <c r="G23" s="99" t="s">
+        <v>63</v>
+      </c>
+      <c r="H23" s="87" t="s">
+        <v>61</v>
+      </c>
+      <c r="I23" s="88" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" ht="30" customHeight="1">
-      <c r="A23" s="52"/>
-      <c r="G23" s="32" t="s">
+      <c r="J23" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="K23" s="87" t="s">
         <v>62</v>
       </c>
-      <c r="H23" s="32" t="s">
+      <c r="L23" s="88" t="s">
         <v>63</v>
       </c>
-      <c r="J23" s="32" t="s">
+      <c r="M23" s="86" t="s">
+        <v>124</v>
+      </c>
+      <c r="N23" s="32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="54"/>
+      <c r="F24" s="86" t="s">
+        <v>125</v>
+      </c>
+      <c r="G24" s="99" t="s">
+        <v>74</v>
+      </c>
+      <c r="J24" s="92"/>
+      <c r="K24" s="92"/>
+      <c r="M24" s="86" t="s">
         <v>69</v>
       </c>
-      <c r="K23" s="33" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" ht="30" customHeight="1">
-      <c r="A24" s="52"/>
-      <c r="J24" s="32" t="s">
+      <c r="N24" s="32" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="55"/>
+      <c r="B25" s="12"/>
+      <c r="F25" s="86" t="s">
+        <v>126</v>
+      </c>
+      <c r="G25" s="99" t="s">
+        <v>75</v>
+      </c>
+      <c r="J25" s="92"/>
+      <c r="K25" s="92"/>
+      <c r="M25" s="86" t="s">
         <v>70</v>
       </c>
-      <c r="K24" s="33" t="s">
+      <c r="N25" s="32" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="30" customHeight="1">
-      <c r="A25" s="53"/>
-      <c r="B25" s="12"/>
-      <c r="J25" s="32" t="s">
+    <row r="26" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="54"/>
+      <c r="F26" s="87" t="s">
         <v>71</v>
       </c>
-      <c r="K25" s="33" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" ht="30" customHeight="1">
-      <c r="A26" s="52"/>
-      <c r="J26" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="K26" s="33" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" ht="30" customHeight="1">
-      <c r="A27" s="52"/>
+      <c r="G26" s="100" t="s">
+        <v>75</v>
+      </c>
+      <c r="J26" s="92"/>
+      <c r="K26" s="92"/>
+      <c r="M26" s="87" t="s">
+        <v>71</v>
+      </c>
+      <c r="N26" s="88" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="54"/>
       <c r="B27" s="11" t="s">
         <v>7</v>
       </c>
       <c r="K27" s="4"/>
     </row>
-    <row r="28" spans="1:14" ht="30" customHeight="1">
-      <c r="A28" s="52"/>
+    <row r="28" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="54"/>
       <c r="K28" s="4"/>
     </row>
-    <row r="29" spans="1:14" ht="30" customHeight="1">
-      <c r="A29" s="52"/>
+    <row r="29" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="54"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
@@ -2147,27 +2296,27 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.6328125" customWidth="1"/>
-    <col min="2" max="2" width="21.81640625" customWidth="1"/>
+    <col min="1" max="1" width="16.625" customWidth="1"/>
+    <col min="2" max="2" width="21.875" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="25.453125" customWidth="1"/>
-    <col min="5" max="5" width="31.08984375" customWidth="1"/>
-    <col min="6" max="6" width="51.36328125" customWidth="1"/>
+    <col min="4" max="4" width="25.5" customWidth="1"/>
+    <col min="5" max="5" width="31.125" customWidth="1"/>
+    <col min="6" max="6" width="51.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="23">
-      <c r="A1" s="69" t="s">
+    <row r="1" spans="1:6" ht="27" x14ac:dyDescent="0.6">
+      <c r="A1" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-    </row>
-    <row r="2" spans="1:6" ht="22.5">
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+    </row>
+    <row r="2" spans="1:6" ht="27" x14ac:dyDescent="0.6">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -2175,53 +2324,53 @@
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
     </row>
-    <row r="3" spans="1:6" ht="23">
+    <row r="3" spans="1:6" ht="27" x14ac:dyDescent="0.6">
       <c r="A3" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="71"/>
+      <c r="B3" s="76"/>
+      <c r="C3" s="77"/>
       <c r="D3" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="72"/>
-      <c r="F3" s="68"/>
-    </row>
-    <row r="4" spans="1:6" ht="23">
+      <c r="E3" s="78"/>
+      <c r="F3" s="74"/>
+    </row>
+    <row r="4" spans="1:6" ht="27" x14ac:dyDescent="0.6">
       <c r="A4" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="66"/>
+      <c r="B4" s="71"/>
+      <c r="C4" s="72"/>
       <c r="D4" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="67"/>
-      <c r="F4" s="68"/>
-    </row>
-    <row r="5" spans="1:6" ht="23">
+      <c r="E4" s="73"/>
+      <c r="F4" s="74"/>
+    </row>
+    <row r="5" spans="1:6" ht="27" x14ac:dyDescent="0.6">
       <c r="A5" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="72"/>
-      <c r="C5" s="67"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="73"/>
       <c r="D5" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="73"/>
-      <c r="F5" s="74"/>
-    </row>
-    <row r="6" spans="1:6" ht="23">
-      <c r="A6" s="75" t="s">
+      <c r="E5" s="79"/>
+      <c r="F5" s="80"/>
+    </row>
+    <row r="6" spans="1:6" ht="27" x14ac:dyDescent="0.6">
+      <c r="A6" s="81" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="75"/>
-      <c r="C6" s="72"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="68"/>
-    </row>
-    <row r="7" spans="1:6" ht="22.5">
+      <c r="B6" s="81"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="73"/>
+      <c r="E6" s="73"/>
+      <c r="F6" s="74"/>
+    </row>
+    <row r="7" spans="1:6" ht="27" x14ac:dyDescent="0.6">
       <c r="A7" s="13"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -2229,7 +2378,7 @@
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
     </row>
-    <row r="8" spans="1:6" ht="39" customHeight="1">
+    <row r="8" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
         <v>31</v>
       </c>
@@ -2249,32 +2398,32 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="22.5">
-      <c r="A9" s="62"/>
+    <row r="9" spans="1:6" ht="27" x14ac:dyDescent="0.6">
+      <c r="A9" s="68"/>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
     </row>
-    <row r="10" spans="1:6" ht="22.5">
-      <c r="A10" s="63"/>
+    <row r="10" spans="1:6" ht="27" x14ac:dyDescent="0.6">
+      <c r="A10" s="69"/>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
     </row>
-    <row r="11" spans="1:6" ht="22.5">
-      <c r="A11" s="63"/>
+    <row r="11" spans="1:6" ht="27" x14ac:dyDescent="0.6">
+      <c r="A11" s="69"/>
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
     </row>
-    <row r="12" spans="1:6" ht="22.5">
-      <c r="A12" s="64"/>
+    <row r="12" spans="1:6" ht="27" x14ac:dyDescent="0.6">
+      <c r="A12" s="70"/>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
@@ -2306,15 +2455,15 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="30" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="30.453125" style="18" customWidth="1"/>
-    <col min="2" max="2" width="31.6328125" style="18" customWidth="1"/>
-    <col min="3" max="3" width="44.08984375" style="18" customWidth="1"/>
-    <col min="4" max="16384" width="10.81640625" style="18"/>
+    <col min="1" max="1" width="30.5" style="18" customWidth="1"/>
+    <col min="2" max="2" width="31.625" style="18" customWidth="1"/>
+    <col min="3" max="3" width="44.125" style="18" customWidth="1"/>
+    <col min="4" max="16384" width="10.875" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" customHeight="1">
+    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A1" s="16" t="s">
         <v>15</v>
       </c>
@@ -2325,51 +2474,51 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" customHeight="1">
+    <row r="2" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A2" s="19"/>
       <c r="B2" s="19"/>
       <c r="C2" s="19"/>
     </row>
-    <row r="3" spans="1:3" ht="30" customHeight="1">
+    <row r="3" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A3" s="19"/>
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
     </row>
-    <row r="4" spans="1:3" ht="30" customHeight="1">
+    <row r="4" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A4" s="19"/>
       <c r="B4" s="19"/>
       <c r="C4" s="19"/>
     </row>
-    <row r="5" spans="1:3" ht="30" customHeight="1">
+    <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A5" s="19"/>
       <c r="B5" s="19"/>
       <c r="C5" s="19"/>
     </row>
-    <row r="6" spans="1:3" ht="30" customHeight="1">
+    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A6" s="19"/>
       <c r="B6" s="19"/>
       <c r="C6" s="19"/>
     </row>
-    <row r="7" spans="1:3" ht="30" customHeight="1">
+    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A7" s="19"/>
       <c r="B7" s="19"/>
       <c r="C7" s="19"/>
     </row>
-    <row r="8" spans="1:3" ht="30" customHeight="1">
+    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A8" s="19"/>
       <c r="B8" s="19"/>
       <c r="C8" s="19"/>
     </row>
-    <row r="9" spans="1:3" ht="30" customHeight="1">
+    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A9" s="19"/>
       <c r="B9" s="19"/>
       <c r="C9" s="19"/>
     </row>
-    <row r="10" spans="1:3" ht="30" customHeight="1">
-      <c r="A10" s="76" t="s">
+    <row r="10" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A10" s="82" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="77"/>
+      <c r="B10" s="83"/>
       <c r="C10" s="20"/>
     </row>
   </sheetData>
@@ -2388,18 +2537,18 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="22.5"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="27" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="16.6328125" style="13" customWidth="1"/>
-    <col min="2" max="2" width="11.6328125" style="13" customWidth="1"/>
-    <col min="3" max="3" width="23.08984375" style="13" customWidth="1"/>
-    <col min="4" max="4" width="27.81640625" style="13" customWidth="1"/>
-    <col min="5" max="5" width="33.81640625" style="13" customWidth="1"/>
-    <col min="6" max="6" width="32.36328125" style="13" customWidth="1"/>
-    <col min="7" max="16384" width="10.81640625" style="13"/>
+    <col min="1" max="1" width="16.625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="11.625" style="13" customWidth="1"/>
+    <col min="3" max="3" width="23.125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="27.875" style="13" customWidth="1"/>
+    <col min="5" max="5" width="33.875" style="13" customWidth="1"/>
+    <col min="6" max="6" width="32.375" style="13" customWidth="1"/>
+    <col min="7" max="16384" width="10.875" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="24" customFormat="1" ht="23">
+    <row r="1" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A1" s="15" t="s">
         <v>37</v>
       </c>
@@ -2419,7 +2568,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.6">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
@@ -2427,7 +2576,7 @@
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.6">
       <c r="A3" s="14"/>
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
@@ -2435,7 +2584,7 @@
       <c r="E3" s="14"/>
       <c r="F3" s="14"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.6">
       <c r="A4" s="14"/>
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
@@ -2443,7 +2592,7 @@
       <c r="E4" s="14"/>
       <c r="F4" s="14"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.6">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
@@ -2451,7 +2600,7 @@
       <c r="E5" s="14"/>
       <c r="F5" s="14"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.6">
       <c r="A6" s="14"/>
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
@@ -2459,7 +2608,7 @@
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.6">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
@@ -2467,7 +2616,7 @@
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.6">
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
@@ -2475,7 +2624,7 @@
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.6">
       <c r="A9" s="14"/>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
@@ -2483,7 +2632,7 @@
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.6">
       <c r="A10" s="14"/>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
@@ -2491,7 +2640,7 @@
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.6">
       <c r="A11" s="14"/>
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
@@ -2499,7 +2648,7 @@
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.6">
       <c r="A12" s="14"/>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
@@ -2507,7 +2656,7 @@
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.6">
       <c r="A13" s="14"/>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
@@ -2515,7 +2664,7 @@
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.6">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>

</xml_diff>

<commit_message>
Update Task Estimation 17/1/69
</commit_message>
<xml_diff>
--- a/Lab_5/ADAPT_Blueprint.xlsx
+++ b/Lab_5/ADAPT_Blueprint.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Lab5SoftEngineer\Lab_5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF846262-17E9-492E-9F30-62785132FAAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3197C99E-A692-451E-B3B3-B36D5BBE4905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{C5F2AE7F-2A01-4E3D-A1FD-0F4756AFC920}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="231">
   <si>
     <t>A-DAPT Blueprint</t>
   </si>
@@ -805,15 +805,6 @@
     <t>TS-010</t>
   </si>
   <si>
-    <t>ออกแบบ Database Schema (ตารางสอบ, วิชา, ห้องสอบ)</t>
-  </si>
-  <si>
-    <t>พัฒนา Public API สำหรับค้นหาตารางสอบตามรหัสวิชา</t>
-  </si>
-  <si>
-    <t>พัฒนา Private API ดึงตารางสอบส่วนตัว (Mapping ข้อมูลลงทะเบียน)</t>
-  </si>
-  <si>
     <t>ระบบ Caching ข้อมูลตารางสอบ (รองรับ Traffic จำนวนมาก)</t>
   </si>
   <si>
@@ -838,32 +829,77 @@
     <t>System Architecture</t>
   </si>
   <si>
-    <t>Backend API</t>
-  </si>
-  <si>
-    <t>Frontend (Public)</t>
-  </si>
-  <si>
-    <t>Frontend (Member)</t>
-  </si>
-  <si>
     <t>Security/Auth</t>
   </si>
   <si>
-    <t>Testing</t>
-  </si>
-  <si>
     <t>Deployment</t>
   </si>
   <si>
-    <t>294 ชั่วโมงต่อ /sprint</t>
+    <t>ประมาณ 294 ชั่วโมงต่อ /sprint</t>
+  </si>
+  <si>
+    <t>ออกแบบ Database Schema (ตารางสอบ, วิชา, ห้องสอบ เป็นต้น) ส่วนของ Login และ ไม่ Login</t>
+  </si>
+  <si>
+    <t>Load Testing</t>
+  </si>
+  <si>
+    <t>Testing Testcase</t>
+  </si>
+  <si>
+    <t>TS-011</t>
+  </si>
+  <si>
+    <t>System Architecture ConstrainKey</t>
+  </si>
+  <si>
+    <t>กำหนด Primary Key,Foreign Key,กำหนด Unique Key เช่น(Room+Date+Time)</t>
+  </si>
+  <si>
+    <t>Test Mock Data</t>
+  </si>
+  <si>
+    <t>เตรียมข้อมูลเพื่อใช้ในการทดสอบต่างๆเช่น ปี วิชา เทอม ตาราง</t>
+  </si>
+  <si>
+    <t xml:space="preserve">พัฒนา Public API สำหรับดึงหรือค้นหาตารางสอบตามรหัสวิชาที่ค้นหาแบบไม่ Login </t>
+  </si>
+  <si>
+    <t>พัฒนา Private API ดึงหรือค้นหาตารางสอบส่วนตัว (Mapping ข้อมูลลงทะเบียน) ที่ได้ลงทะเบียนไป</t>
+  </si>
+  <si>
+    <t>Make public API table</t>
+  </si>
+  <si>
+    <t>Make private API table</t>
+  </si>
+  <si>
+    <t>TS-012</t>
+  </si>
+  <si>
+    <t>TS-013</t>
+  </si>
+  <si>
+    <t>Frontend (Login)</t>
+  </si>
+  <si>
+    <t>Frontend (No Login)</t>
+  </si>
+  <si>
+    <t>Task Enrolled Table</t>
+  </si>
+  <si>
+    <t>ทำเกี่ยวกับการดึงข้อมูล ตารางเรียนของผู้ Login มาแสดงในหน้า</t>
+  </si>
+  <si>
+    <t>Backend Support API</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -990,6 +1026,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -1313,7 +1356,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1508,6 +1551,63 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1538,78 +1638,23 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2834,7 +2879,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BA8F482-35D4-7F4D-A673-99B751C602BA}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView zoomScale="66" workbookViewId="0">
+    <sheetView topLeftCell="A14" zoomScale="66" workbookViewId="0">
       <selection activeCell="E41" sqref="E41:E49"/>
     </sheetView>
   </sheetViews>
@@ -2849,14 +2894,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25">
-      <c r="A1" s="113" t="s">
+      <c r="A1" s="98" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="113"/>
-      <c r="C1" s="113"/>
-      <c r="D1" s="113"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="113"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
     </row>
     <row r="2" spans="1:6" ht="23.25">
       <c r="A2" s="13"/>
@@ -2870,53 +2915,53 @@
       <c r="A3" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="114" t="s">
+      <c r="B3" s="99" t="s">
         <v>145</v>
       </c>
-      <c r="C3" s="115"/>
+      <c r="C3" s="100"/>
       <c r="D3" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="116"/>
-      <c r="F3" s="117"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="93"/>
     </row>
     <row r="4" spans="1:6" ht="25.5">
       <c r="A4" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="109"/>
-      <c r="C4" s="110"/>
+      <c r="B4" s="94"/>
+      <c r="C4" s="95"/>
       <c r="D4" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="111" t="s">
+      <c r="E4" s="96" t="s">
         <v>146</v>
       </c>
-      <c r="F4" s="112"/>
+      <c r="F4" s="97"/>
     </row>
     <row r="5" spans="1:6" ht="23.25">
       <c r="A5" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="116"/>
-      <c r="C5" s="118"/>
+      <c r="B5" s="88"/>
+      <c r="C5" s="89"/>
       <c r="D5" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="119" t="s">
+      <c r="E5" s="90" t="s">
         <v>147</v>
       </c>
-      <c r="F5" s="120"/>
+      <c r="F5" s="91"/>
     </row>
     <row r="6" spans="1:6" ht="23.25">
-      <c r="A6" s="121" t="s">
+      <c r="A6" s="92" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="121"/>
-      <c r="C6" s="116"/>
-      <c r="D6" s="118"/>
-      <c r="E6" s="118"/>
-      <c r="F6" s="117"/>
+      <c r="B6" s="92"/>
+      <c r="C6" s="88"/>
+      <c r="D6" s="89"/>
+      <c r="E6" s="89"/>
+      <c r="F6" s="93"/>
     </row>
     <row r="7" spans="1:6" ht="23.25">
       <c r="A7" s="13"/>
@@ -2947,10 +2992,10 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="34.9" customHeight="1">
-      <c r="A9" s="103" t="s">
+      <c r="A9" s="101" t="s">
         <v>144</v>
       </c>
-      <c r="B9" s="94" t="s">
+      <c r="B9" s="113" t="s">
         <v>150</v>
       </c>
       <c r="C9" s="68" t="s">
@@ -2963,8 +3008,8 @@
       <c r="F9" s="67"/>
     </row>
     <row r="10" spans="1:6" ht="72">
-      <c r="A10" s="104"/>
-      <c r="B10" s="95"/>
+      <c r="A10" s="102"/>
+      <c r="B10" s="114"/>
       <c r="C10" s="69" t="s">
         <v>151</v>
       </c>
@@ -2975,8 +3020,8 @@
       <c r="F10" s="67"/>
     </row>
     <row r="11" spans="1:6" ht="72">
-      <c r="A11" s="104"/>
-      <c r="B11" s="95"/>
+      <c r="A11" s="102"/>
+      <c r="B11" s="114"/>
       <c r="C11" s="68" t="s">
         <v>159</v>
       </c>
@@ -2987,28 +3032,28 @@
       <c r="F11" s="67"/>
     </row>
     <row r="12" spans="1:6" ht="17.45" customHeight="1">
-      <c r="A12" s="104"/>
-      <c r="B12" s="95"/>
-      <c r="C12" s="97" t="s">
+      <c r="A12" s="102"/>
+      <c r="B12" s="114"/>
+      <c r="C12" s="116" t="s">
         <v>155</v>
       </c>
-      <c r="D12" s="97" t="s">
+      <c r="D12" s="116" t="s">
         <v>156</v>
       </c>
-      <c r="E12" s="100"/>
-      <c r="F12" s="100"/>
+      <c r="E12" s="118"/>
+      <c r="F12" s="118"/>
     </row>
     <row r="13" spans="1:6" ht="69.599999999999994" customHeight="1">
-      <c r="A13" s="104"/>
-      <c r="B13" s="95"/>
-      <c r="C13" s="99"/>
-      <c r="D13" s="99"/>
-      <c r="E13" s="102"/>
-      <c r="F13" s="102"/>
+      <c r="A13" s="102"/>
+      <c r="B13" s="114"/>
+      <c r="C13" s="117"/>
+      <c r="D13" s="117"/>
+      <c r="E13" s="119"/>
+      <c r="F13" s="119"/>
     </row>
     <row r="14" spans="1:6" ht="72">
-      <c r="A14" s="104"/>
-      <c r="B14" s="95"/>
+      <c r="A14" s="102"/>
+      <c r="B14" s="114"/>
       <c r="C14" s="68" t="s">
         <v>157</v>
       </c>
@@ -3019,8 +3064,8 @@
       <c r="F14" s="67"/>
     </row>
     <row r="15" spans="1:6" ht="90">
-      <c r="A15" s="104"/>
-      <c r="B15" s="95"/>
+      <c r="A15" s="102"/>
+      <c r="B15" s="114"/>
       <c r="C15" s="68" t="s">
         <v>160</v>
       </c>
@@ -3031,106 +3076,106 @@
       <c r="F15" s="67"/>
     </row>
     <row r="16" spans="1:6" ht="17.45" customHeight="1">
-      <c r="A16" s="104"/>
-      <c r="B16" s="95"/>
-      <c r="C16" s="106" t="s">
+      <c r="A16" s="102"/>
+      <c r="B16" s="114"/>
+      <c r="C16" s="104" t="s">
         <v>162</v>
       </c>
-      <c r="D16" s="88" t="s">
+      <c r="D16" s="107" t="s">
         <v>163</v>
       </c>
-      <c r="E16" s="91"/>
-      <c r="F16" s="91"/>
+      <c r="E16" s="110"/>
+      <c r="F16" s="110"/>
     </row>
     <row r="17" spans="1:6" ht="52.15" customHeight="1">
-      <c r="A17" s="104"/>
-      <c r="B17" s="95"/>
-      <c r="C17" s="108"/>
-      <c r="D17" s="90"/>
-      <c r="E17" s="93"/>
-      <c r="F17" s="93"/>
+      <c r="A17" s="102"/>
+      <c r="B17" s="114"/>
+      <c r="C17" s="106"/>
+      <c r="D17" s="109"/>
+      <c r="E17" s="112"/>
+      <c r="F17" s="112"/>
     </row>
     <row r="18" spans="1:6" ht="14.45" customHeight="1">
-      <c r="A18" s="104"/>
-      <c r="B18" s="95"/>
-      <c r="C18" s="106" t="s">
+      <c r="A18" s="102"/>
+      <c r="B18" s="114"/>
+      <c r="C18" s="104" t="s">
         <v>164</v>
       </c>
-      <c r="D18" s="88" t="s">
+      <c r="D18" s="107" t="s">
         <v>165</v>
       </c>
-      <c r="E18" s="91"/>
-      <c r="F18" s="91"/>
+      <c r="E18" s="110"/>
+      <c r="F18" s="110"/>
     </row>
     <row r="19" spans="1:6" ht="14.45" customHeight="1">
-      <c r="A19" s="104"/>
-      <c r="B19" s="95"/>
-      <c r="C19" s="107"/>
-      <c r="D19" s="89"/>
-      <c r="E19" s="92"/>
-      <c r="F19" s="92"/>
+      <c r="A19" s="102"/>
+      <c r="B19" s="114"/>
+      <c r="C19" s="105"/>
+      <c r="D19" s="108"/>
+      <c r="E19" s="111"/>
+      <c r="F19" s="111"/>
     </row>
     <row r="20" spans="1:6" ht="14.45" customHeight="1">
-      <c r="A20" s="104"/>
-      <c r="B20" s="95"/>
-      <c r="C20" s="107"/>
-      <c r="D20" s="89"/>
-      <c r="E20" s="92"/>
-      <c r="F20" s="92"/>
+      <c r="A20" s="102"/>
+      <c r="B20" s="114"/>
+      <c r="C20" s="105"/>
+      <c r="D20" s="108"/>
+      <c r="E20" s="111"/>
+      <c r="F20" s="111"/>
     </row>
     <row r="21" spans="1:6" ht="14.45" customHeight="1">
-      <c r="A21" s="104"/>
-      <c r="B21" s="95"/>
-      <c r="C21" s="107"/>
-      <c r="D21" s="89"/>
-      <c r="E21" s="92"/>
-      <c r="F21" s="92"/>
+      <c r="A21" s="102"/>
+      <c r="B21" s="114"/>
+      <c r="C21" s="105"/>
+      <c r="D21" s="108"/>
+      <c r="E21" s="111"/>
+      <c r="F21" s="111"/>
     </row>
     <row r="22" spans="1:6" ht="17.45" customHeight="1">
-      <c r="A22" s="104"/>
-      <c r="B22" s="95"/>
-      <c r="C22" s="107"/>
-      <c r="D22" s="89"/>
-      <c r="E22" s="92"/>
-      <c r="F22" s="92"/>
+      <c r="A22" s="102"/>
+      <c r="B22" s="114"/>
+      <c r="C22" s="105"/>
+      <c r="D22" s="108"/>
+      <c r="E22" s="111"/>
+      <c r="F22" s="111"/>
     </row>
     <row r="23" spans="1:6" ht="17.45" customHeight="1">
-      <c r="A23" s="104"/>
-      <c r="B23" s="95"/>
-      <c r="C23" s="107"/>
-      <c r="D23" s="89"/>
-      <c r="E23" s="92"/>
-      <c r="F23" s="92"/>
+      <c r="A23" s="102"/>
+      <c r="B23" s="114"/>
+      <c r="C23" s="105"/>
+      <c r="D23" s="108"/>
+      <c r="E23" s="111"/>
+      <c r="F23" s="111"/>
     </row>
     <row r="24" spans="1:6" ht="17.45" customHeight="1">
-      <c r="A24" s="104"/>
-      <c r="B24" s="95"/>
-      <c r="C24" s="107"/>
-      <c r="D24" s="89"/>
-      <c r="E24" s="92"/>
-      <c r="F24" s="92"/>
+      <c r="A24" s="102"/>
+      <c r="B24" s="114"/>
+      <c r="C24" s="105"/>
+      <c r="D24" s="108"/>
+      <c r="E24" s="111"/>
+      <c r="F24" s="111"/>
     </row>
     <row r="25" spans="1:6" ht="17.45" customHeight="1">
-      <c r="A25" s="104"/>
-      <c r="B25" s="95"/>
-      <c r="C25" s="107"/>
-      <c r="D25" s="89"/>
-      <c r="E25" s="92"/>
-      <c r="F25" s="92"/>
+      <c r="A25" s="102"/>
+      <c r="B25" s="114"/>
+      <c r="C25" s="105"/>
+      <c r="D25" s="108"/>
+      <c r="E25" s="111"/>
+      <c r="F25" s="111"/>
     </row>
     <row r="26" spans="1:6" ht="20.45" customHeight="1">
-      <c r="A26" s="105"/>
-      <c r="B26" s="96"/>
-      <c r="C26" s="108"/>
-      <c r="D26" s="90"/>
-      <c r="E26" s="93"/>
-      <c r="F26" s="93"/>
+      <c r="A26" s="103"/>
+      <c r="B26" s="115"/>
+      <c r="C26" s="106"/>
+      <c r="D26" s="109"/>
+      <c r="E26" s="112"/>
+      <c r="F26" s="112"/>
     </row>
     <row r="27" spans="1:6" ht="36">
-      <c r="A27" s="103" t="s">
+      <c r="A27" s="101" t="s">
         <v>166</v>
       </c>
-      <c r="B27" s="94" t="s">
+      <c r="B27" s="113" t="s">
         <v>154</v>
       </c>
       <c r="C27" s="68" t="s">
@@ -3142,9 +3187,9 @@
       <c r="E27" s="67"/>
       <c r="F27" s="67"/>
     </row>
-    <row r="28" spans="1:6" ht="72">
-      <c r="A28" s="104"/>
-      <c r="B28" s="95"/>
+    <row r="28" spans="1:6" ht="54">
+      <c r="A28" s="102"/>
+      <c r="B28" s="114"/>
       <c r="C28" s="69" t="s">
         <v>167</v>
       </c>
@@ -3155,8 +3200,8 @@
       <c r="F28" s="67"/>
     </row>
     <row r="29" spans="1:6" ht="90">
-      <c r="A29" s="104"/>
-      <c r="B29" s="95"/>
+      <c r="A29" s="102"/>
+      <c r="B29" s="114"/>
       <c r="C29" s="68" t="s">
         <v>171</v>
       </c>
@@ -3167,185 +3212,194 @@
       <c r="F29" s="67"/>
     </row>
     <row r="30" spans="1:6" ht="17.45" customHeight="1">
-      <c r="A30" s="104"/>
-      <c r="B30" s="95"/>
-      <c r="C30" s="97" t="s">
+      <c r="A30" s="102"/>
+      <c r="B30" s="114"/>
+      <c r="C30" s="116" t="s">
         <v>170</v>
       </c>
-      <c r="D30" s="97" t="s">
+      <c r="D30" s="116" t="s">
         <v>172</v>
       </c>
-      <c r="E30" s="100"/>
-      <c r="F30" s="100"/>
+      <c r="E30" s="118"/>
+      <c r="F30" s="118"/>
     </row>
     <row r="31" spans="1:6" ht="17.45" customHeight="1">
-      <c r="A31" s="104"/>
-      <c r="B31" s="95"/>
-      <c r="C31" s="98"/>
-      <c r="D31" s="98"/>
-      <c r="E31" s="101"/>
-      <c r="F31" s="101"/>
+      <c r="A31" s="102"/>
+      <c r="B31" s="114"/>
+      <c r="C31" s="120"/>
+      <c r="D31" s="120"/>
+      <c r="E31" s="121"/>
+      <c r="F31" s="121"/>
     </row>
     <row r="32" spans="1:6" ht="17.45" customHeight="1">
-      <c r="A32" s="104"/>
-      <c r="B32" s="95"/>
-      <c r="C32" s="98"/>
-      <c r="D32" s="98"/>
-      <c r="E32" s="101"/>
-      <c r="F32" s="101"/>
+      <c r="A32" s="102"/>
+      <c r="B32" s="114"/>
+      <c r="C32" s="120"/>
+      <c r="D32" s="120"/>
+      <c r="E32" s="121"/>
+      <c r="F32" s="121"/>
     </row>
     <row r="33" spans="1:6" ht="17.45" customHeight="1">
-      <c r="A33" s="104"/>
-      <c r="B33" s="95"/>
-      <c r="C33" s="98"/>
-      <c r="D33" s="98"/>
-      <c r="E33" s="101"/>
-      <c r="F33" s="101"/>
+      <c r="A33" s="102"/>
+      <c r="B33" s="114"/>
+      <c r="C33" s="120"/>
+      <c r="D33" s="120"/>
+      <c r="E33" s="121"/>
+      <c r="F33" s="121"/>
     </row>
     <row r="34" spans="1:6" ht="14.45" customHeight="1">
-      <c r="A34" s="104"/>
-      <c r="B34" s="95"/>
-      <c r="C34" s="99"/>
-      <c r="D34" s="99"/>
-      <c r="E34" s="102"/>
-      <c r="F34" s="102"/>
+      <c r="A34" s="102"/>
+      <c r="B34" s="114"/>
+      <c r="C34" s="117"/>
+      <c r="D34" s="117"/>
+      <c r="E34" s="119"/>
+      <c r="F34" s="119"/>
     </row>
     <row r="35" spans="1:6" ht="14.45" customHeight="1">
-      <c r="A35" s="104"/>
-      <c r="B35" s="95"/>
-      <c r="C35" s="97" t="s">
+      <c r="A35" s="102"/>
+      <c r="B35" s="114"/>
+      <c r="C35" s="116" t="s">
         <v>173</v>
       </c>
-      <c r="D35" s="97" t="s">
+      <c r="D35" s="116" t="s">
         <v>174</v>
       </c>
-      <c r="E35" s="91"/>
-      <c r="F35" s="91"/>
+      <c r="E35" s="110"/>
+      <c r="F35" s="110"/>
     </row>
     <row r="36" spans="1:6" ht="14.45" customHeight="1">
-      <c r="A36" s="104"/>
-      <c r="B36" s="95"/>
-      <c r="C36" s="98"/>
-      <c r="D36" s="98"/>
-      <c r="E36" s="92"/>
-      <c r="F36" s="92"/>
+      <c r="A36" s="102"/>
+      <c r="B36" s="114"/>
+      <c r="C36" s="120"/>
+      <c r="D36" s="120"/>
+      <c r="E36" s="111"/>
+      <c r="F36" s="111"/>
     </row>
     <row r="37" spans="1:6" ht="14.45" customHeight="1">
-      <c r="A37" s="104"/>
-      <c r="B37" s="95"/>
-      <c r="C37" s="98"/>
-      <c r="D37" s="98"/>
-      <c r="E37" s="92"/>
-      <c r="F37" s="92"/>
+      <c r="A37" s="102"/>
+      <c r="B37" s="114"/>
+      <c r="C37" s="120"/>
+      <c r="D37" s="120"/>
+      <c r="E37" s="111"/>
+      <c r="F37" s="111"/>
     </row>
     <row r="38" spans="1:6" ht="14.45" customHeight="1">
-      <c r="A38" s="104"/>
-      <c r="B38" s="95"/>
-      <c r="C38" s="98"/>
-      <c r="D38" s="98"/>
-      <c r="E38" s="92"/>
-      <c r="F38" s="92"/>
+      <c r="A38" s="102"/>
+      <c r="B38" s="114"/>
+      <c r="C38" s="120"/>
+      <c r="D38" s="120"/>
+      <c r="E38" s="111"/>
+      <c r="F38" s="111"/>
     </row>
     <row r="39" spans="1:6" ht="14.45" customHeight="1">
-      <c r="A39" s="104"/>
-      <c r="B39" s="95"/>
-      <c r="C39" s="98"/>
-      <c r="D39" s="98"/>
-      <c r="E39" s="92"/>
-      <c r="F39" s="92"/>
+      <c r="A39" s="102"/>
+      <c r="B39" s="114"/>
+      <c r="C39" s="120"/>
+      <c r="D39" s="120"/>
+      <c r="E39" s="111"/>
+      <c r="F39" s="111"/>
     </row>
     <row r="40" spans="1:6" ht="14.45" customHeight="1">
-      <c r="A40" s="104"/>
-      <c r="B40" s="95"/>
-      <c r="C40" s="99"/>
-      <c r="D40" s="99"/>
-      <c r="E40" s="93"/>
-      <c r="F40" s="93"/>
+      <c r="A40" s="102"/>
+      <c r="B40" s="114"/>
+      <c r="C40" s="117"/>
+      <c r="D40" s="117"/>
+      <c r="E40" s="112"/>
+      <c r="F40" s="112"/>
     </row>
     <row r="41" spans="1:6" ht="14.45" customHeight="1">
-      <c r="A41" s="104"/>
-      <c r="B41" s="95"/>
-      <c r="C41" s="88" t="s">
+      <c r="A41" s="102"/>
+      <c r="B41" s="114"/>
+      <c r="C41" s="107" t="s">
         <v>176</v>
       </c>
-      <c r="D41" s="88" t="s">
+      <c r="D41" s="107" t="s">
         <v>175</v>
       </c>
-      <c r="E41" s="91"/>
-      <c r="F41" s="91"/>
+      <c r="E41" s="110"/>
+      <c r="F41" s="110"/>
     </row>
     <row r="42" spans="1:6" ht="14.45" customHeight="1">
-      <c r="A42" s="104"/>
-      <c r="B42" s="95"/>
-      <c r="C42" s="89"/>
-      <c r="D42" s="89"/>
-      <c r="E42" s="92"/>
-      <c r="F42" s="92"/>
+      <c r="A42" s="102"/>
+      <c r="B42" s="114"/>
+      <c r="C42" s="108"/>
+      <c r="D42" s="108"/>
+      <c r="E42" s="111"/>
+      <c r="F42" s="111"/>
     </row>
     <row r="43" spans="1:6" ht="14.45" customHeight="1">
-      <c r="A43" s="104"/>
-      <c r="B43" s="95"/>
-      <c r="C43" s="89"/>
-      <c r="D43" s="89"/>
-      <c r="E43" s="92"/>
-      <c r="F43" s="92"/>
+      <c r="A43" s="102"/>
+      <c r="B43" s="114"/>
+      <c r="C43" s="108"/>
+      <c r="D43" s="108"/>
+      <c r="E43" s="111"/>
+      <c r="F43" s="111"/>
     </row>
     <row r="44" spans="1:6" ht="14.45" customHeight="1">
-      <c r="A44" s="104"/>
-      <c r="B44" s="95"/>
-      <c r="C44" s="89"/>
-      <c r="D44" s="89"/>
-      <c r="E44" s="92"/>
-      <c r="F44" s="92"/>
+      <c r="A44" s="102"/>
+      <c r="B44" s="114"/>
+      <c r="C44" s="108"/>
+      <c r="D44" s="108"/>
+      <c r="E44" s="111"/>
+      <c r="F44" s="111"/>
     </row>
     <row r="45" spans="1:6" ht="14.45" customHeight="1">
-      <c r="A45" s="104"/>
-      <c r="B45" s="95"/>
-      <c r="C45" s="89"/>
-      <c r="D45" s="89"/>
-      <c r="E45" s="92"/>
-      <c r="F45" s="92"/>
+      <c r="A45" s="102"/>
+      <c r="B45" s="114"/>
+      <c r="C45" s="108"/>
+      <c r="D45" s="108"/>
+      <c r="E45" s="111"/>
+      <c r="F45" s="111"/>
     </row>
     <row r="46" spans="1:6" ht="14.45" customHeight="1">
-      <c r="A46" s="104"/>
-      <c r="B46" s="95"/>
-      <c r="C46" s="89"/>
-      <c r="D46" s="89"/>
-      <c r="E46" s="92"/>
-      <c r="F46" s="92"/>
+      <c r="A46" s="102"/>
+      <c r="B46" s="114"/>
+      <c r="C46" s="108"/>
+      <c r="D46" s="108"/>
+      <c r="E46" s="111"/>
+      <c r="F46" s="111"/>
     </row>
     <row r="47" spans="1:6" ht="14.45" customHeight="1">
-      <c r="A47" s="104"/>
-      <c r="B47" s="95"/>
-      <c r="C47" s="89"/>
-      <c r="D47" s="89"/>
-      <c r="E47" s="92"/>
-      <c r="F47" s="92"/>
+      <c r="A47" s="102"/>
+      <c r="B47" s="114"/>
+      <c r="C47" s="108"/>
+      <c r="D47" s="108"/>
+      <c r="E47" s="111"/>
+      <c r="F47" s="111"/>
     </row>
     <row r="48" spans="1:6" ht="17.45" customHeight="1">
-      <c r="A48" s="104"/>
-      <c r="B48" s="95"/>
-      <c r="C48" s="89"/>
-      <c r="D48" s="89"/>
-      <c r="E48" s="92"/>
-      <c r="F48" s="92"/>
+      <c r="A48" s="102"/>
+      <c r="B48" s="114"/>
+      <c r="C48" s="108"/>
+      <c r="D48" s="108"/>
+      <c r="E48" s="111"/>
+      <c r="F48" s="111"/>
     </row>
     <row r="49" spans="1:6" ht="17.45" customHeight="1">
-      <c r="A49" s="105"/>
-      <c r="B49" s="96"/>
-      <c r="C49" s="90"/>
-      <c r="D49" s="90"/>
-      <c r="E49" s="93"/>
-      <c r="F49" s="93"/>
+      <c r="A49" s="103"/>
+      <c r="B49" s="115"/>
+      <c r="C49" s="109"/>
+      <c r="D49" s="109"/>
+      <c r="E49" s="112"/>
+      <c r="F49" s="112"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="F41:F49"/>
+    <mergeCell ref="B27:B49"/>
+    <mergeCell ref="C30:C34"/>
+    <mergeCell ref="D30:D34"/>
+    <mergeCell ref="E30:E34"/>
+    <mergeCell ref="F30:F34"/>
+    <mergeCell ref="C35:C40"/>
+    <mergeCell ref="D35:D40"/>
+    <mergeCell ref="E35:E40"/>
+    <mergeCell ref="F35:F40"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="C41:C49"/>
+    <mergeCell ref="D41:D49"/>
+    <mergeCell ref="E41:E49"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="E3:F3"/>
@@ -3362,21 +3416,12 @@
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
     <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="C41:C49"/>
-    <mergeCell ref="D41:D49"/>
-    <mergeCell ref="E41:E49"/>
-    <mergeCell ref="F41:F49"/>
-    <mergeCell ref="B27:B49"/>
-    <mergeCell ref="C30:C34"/>
-    <mergeCell ref="D30:D34"/>
-    <mergeCell ref="E30:E34"/>
-    <mergeCell ref="F30:F34"/>
-    <mergeCell ref="C35:C40"/>
-    <mergeCell ref="D35:D40"/>
-    <mergeCell ref="E35:E40"/>
-    <mergeCell ref="F35:F40"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:F4"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3388,7 +3433,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="30" customHeight="1"/>
@@ -3504,7 +3549,7 @@
     </row>
     <row r="11" spans="1:3" ht="30" customHeight="1">
       <c r="C11" s="18" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -3520,7 +3565,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="23.25"/>
@@ -3560,13 +3605,13 @@
         <v>191</v>
       </c>
       <c r="C2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D2" t="s">
-        <v>201</v>
+        <v>212</v>
       </c>
       <c r="E2" s="14">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F2" s="14">
         <v>1</v>
@@ -3574,32 +3619,32 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="14"/>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="C3" t="s">
-        <v>212</v>
-      </c>
-      <c r="D3" t="s">
-        <v>202</v>
-      </c>
-      <c r="E3" s="14">
-        <v>8</v>
-      </c>
-      <c r="F3" s="14">
+      <c r="C3" s="124" t="s">
+        <v>216</v>
+      </c>
+      <c r="D3" s="125" t="s">
+        <v>217</v>
+      </c>
+      <c r="E3" s="13">
+        <v>4</v>
+      </c>
+      <c r="F3" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="14"/>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="13" t="s">
         <v>193</v>
       </c>
       <c r="C4" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="D4" t="s">
-        <v>203</v>
+        <v>220</v>
       </c>
       <c r="E4" s="14">
         <v>8</v>
@@ -3610,153 +3655,183 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="14"/>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>194</v>
       </c>
       <c r="C5" t="s">
-        <v>212</v>
+        <v>223</v>
       </c>
       <c r="D5" t="s">
-        <v>204</v>
+        <v>221</v>
       </c>
       <c r="E5" s="14">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F5" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="14"/>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="C6" t="s">
-        <v>213</v>
-      </c>
-      <c r="D6" t="s">
-        <v>207</v>
-      </c>
-      <c r="E6" s="14">
-        <v>8</v>
-      </c>
-      <c r="F6" s="14">
-        <v>1</v>
+      <c r="C6" s="125" t="s">
+        <v>228</v>
+      </c>
+      <c r="D6" s="125" t="s">
+        <v>229</v>
+      </c>
+      <c r="E6" s="13">
+        <v>4</v>
+      </c>
+      <c r="F6" s="13">
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="14"/>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="13" t="s">
         <v>196</v>
       </c>
       <c r="C7" t="s">
-        <v>214</v>
+        <v>230</v>
       </c>
       <c r="D7" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="E7" s="14">
         <v>6</v>
       </c>
       <c r="F7" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="14"/>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>197</v>
       </c>
       <c r="C8" t="s">
-        <v>215</v>
+        <v>227</v>
       </c>
       <c r="D8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E8" s="14">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F8" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="14"/>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>198</v>
       </c>
       <c r="C9" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="D9" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="E9" s="14">
         <v>6</v>
       </c>
       <c r="F9" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="14"/>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="C10" t="s">
-        <v>216</v>
-      </c>
-      <c r="D10" t="s">
-        <v>209</v>
-      </c>
-      <c r="E10" s="14">
-        <v>6</v>
-      </c>
-      <c r="F10" s="14">
+      <c r="C10" s="125" t="s">
+        <v>218</v>
+      </c>
+      <c r="D10" s="125" t="s">
+        <v>219</v>
+      </c>
+      <c r="E10" s="13">
+        <v>1</v>
+      </c>
+      <c r="F10" s="13">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="14"/>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="13" t="s">
         <v>200</v>
       </c>
       <c r="C11" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="D11" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="E11" s="14">
         <v>4</v>
       </c>
       <c r="F11" s="14">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
+      <c r="B12" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="C12" t="s">
+        <v>213</v>
+      </c>
+      <c r="D12" t="s">
+        <v>205</v>
+      </c>
+      <c r="E12" s="14">
+        <v>6</v>
+      </c>
+      <c r="F12" s="14">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
+      <c r="B13" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="C13" t="s">
+        <v>214</v>
+      </c>
+      <c r="D13" t="s">
+        <v>206</v>
+      </c>
+      <c r="E13" s="14">
+        <v>6</v>
+      </c>
+      <c r="F13" s="14">
+        <v>3</v>
+      </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
+      <c r="B14" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="C14" t="s">
+        <v>210</v>
+      </c>
+      <c r="D14" t="s">
+        <v>207</v>
+      </c>
+      <c r="E14" s="14">
+        <v>4</v>
+      </c>
+      <c r="F14" s="14">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>

</xml_diff>